<commit_message>
Largest and the latest version V.12???
</commit_message>
<xml_diff>
--- a/SPC.v5/Docs/Project Diary Template.xlsx
+++ b/SPC.v5/Docs/Project Diary Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\College\College\Third year\SPC\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\College\College\Third year\SPC\phpAssingment\SPC.v5\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="67">
   <si>
     <t>Project Diary</t>
   </si>
@@ -66,9 +66,6 @@
   </si>
   <si>
     <t>23rd</t>
-  </si>
-  <si>
-    <t>6h</t>
   </si>
   <si>
     <t>Login research</t>
@@ -377,7 +374,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -423,6 +420,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -450,16 +459,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -779,7 +779,7 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20:F20"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -794,32 +794,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="19"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="23"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="20"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="22"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="26"/>
     </row>
     <row r="3" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
@@ -834,17 +834,17 @@
       <c r="D3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23" t="s">
+      <c r="F3" s="27"/>
+      <c r="G3" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -859,17 +859,17 @@
       <c r="D4" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="28"/>
-      <c r="G4" s="26" t="s">
+      <c r="F4" s="19"/>
+      <c r="G4" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
-      <c r="K4" s="27"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="18"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
@@ -879,436 +879,440 @@
         <v>8</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="E5" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="19"/>
+      <c r="G5" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="28"/>
-      <c r="G5" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="27"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="18"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="E6" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="19"/>
+      <c r="G6" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="28"/>
-      <c r="G6" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
-      <c r="K6" s="27"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="18"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="C7" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="D7" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="E7" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="19"/>
+      <c r="G7" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="28"/>
-      <c r="G7" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="27"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="18"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="C8" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>23</v>
-      </c>
       <c r="D8" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="19"/>
+      <c r="G8" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="28"/>
-      <c r="G8" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="27"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="18"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="C9" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="D9" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="E9" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="19"/>
+      <c r="G9" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="28"/>
-      <c r="G9" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="26"/>
-      <c r="K9" s="27"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="18"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="11" t="s">
+      <c r="E10" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="19"/>
+      <c r="G10" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="28"/>
-      <c r="G10" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="26"/>
-      <c r="K10" s="27"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="18"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D11" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="19"/>
+      <c r="G11" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="28"/>
-      <c r="G11" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="27"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="18"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="19"/>
+      <c r="G12" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" s="28"/>
-      <c r="G12" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="26"/>
-      <c r="K12" s="27"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="18"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="12" t="s">
+      <c r="E13" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="19"/>
+      <c r="G13" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="28"/>
-      <c r="G13" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="26"/>
-      <c r="K13" s="27"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="18"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="C14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="E14" s="28" t="s">
+      <c r="E14" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="19"/>
+      <c r="G14" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="F14" s="28"/>
-      <c r="G14" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="26"/>
-      <c r="K14" s="27"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="18"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D15" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="19"/>
+      <c r="G15" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="E15" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="F15" s="28"/>
-      <c r="G15" s="26" t="s">
-        <v>51</v>
-      </c>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="26"/>
-      <c r="K15" s="27"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="18"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D16" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16" s="19"/>
+      <c r="G16" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="E16" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="F16" s="28"/>
-      <c r="G16" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
-      <c r="K16" s="27"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="18"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D17" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="F17" s="19"/>
+      <c r="G17" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="E17" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="F17" s="28"/>
-      <c r="G17" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26"/>
-      <c r="K17" s="27"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="18"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B18" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18" s="3" t="s">
+      <c r="D18" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="E18" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="F18" s="19"/>
+      <c r="G18" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="E18" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="F18" s="28"/>
-      <c r="G18" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
-      <c r="K18" s="27"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="18"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="C19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19" s="12" t="s">
+      <c r="E19" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="19"/>
+      <c r="G19" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="E19" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="F19" s="28"/>
-      <c r="G19" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="H19" s="26"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="26"/>
-      <c r="K19" s="27"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="18"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B20" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="C20" s="3" t="s">
+      <c r="D20" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="E20" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="F20" s="19"/>
+      <c r="G20" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="E20" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="F20" s="28"/>
-      <c r="G20" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="H20" s="26"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
-      <c r="K20" s="27"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="18"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="14"/>
+      <c r="A21" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>60</v>
+      </c>
       <c r="C21" s="3"/>
       <c r="D21" s="12"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="26"/>
-      <c r="J21" s="26"/>
-      <c r="K21" s="27"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="18"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="14"/>
       <c r="C22" s="3"/>
       <c r="D22" s="12"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="26"/>
-      <c r="J22" s="26"/>
-      <c r="K22" s="27"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="17"/>
+      <c r="K22" s="18"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="16"/>
       <c r="B23" s="15"/>
       <c r="C23" s="2"/>
       <c r="D23" s="13"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="24"/>
-      <c r="I23" s="24"/>
-      <c r="J23" s="24"/>
-      <c r="K23" s="25"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="28"/>
+      <c r="I23" s="28"/>
+      <c r="J23" s="28"/>
+      <c r="K23" s="29"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G24" s="10"/>
@@ -1326,33 +1330,6 @@
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="G11:K11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G10:K10"/>
-    <mergeCell ref="G9:K9"/>
-    <mergeCell ref="G8:K8"/>
-    <mergeCell ref="G7:K7"/>
-    <mergeCell ref="G6:K6"/>
-    <mergeCell ref="G5:K5"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E7:F7"/>
     <mergeCell ref="A1:K2"/>
     <mergeCell ref="G3:K3"/>
     <mergeCell ref="E3:F3"/>
@@ -1369,6 +1346,33 @@
     <mergeCell ref="G13:K13"/>
     <mergeCell ref="G12:K12"/>
     <mergeCell ref="G4:K4"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G10:K10"/>
+    <mergeCell ref="G9:K9"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="G7:K7"/>
+    <mergeCell ref="G6:K6"/>
+    <mergeCell ref="G5:K5"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G11:K11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>